<commit_message>
Add Q&A.md; Change rules; Delete outdated rules; Update logs
</commit_message>
<xml_diff>
--- a/tex/参数表new_.xlsx
+++ b/tex/参数表new_.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB22655-E775-418F-AD9A-503AC3897AAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A8996-A691-4989-A85A-36634A3A21DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4764" yWindow="120" windowWidth="16152" windowHeight="8508" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5832" yWindow="120" windowWidth="16152" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -819,110 +819,110 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,25 +1264,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M117"/>
   <sheetViews>
-    <sheetView topLeftCell="E76" workbookViewId="0">
-      <selection activeCell="I87" sqref="I87:M101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="A7:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.3125" customWidth="1"/>
+    <col min="2" max="2" width="21.20703125" customWidth="1"/>
+    <col min="3" max="3" width="32.3125" customWidth="1"/>
+    <col min="4" max="4" width="20.41796875" customWidth="1"/>
+    <col min="5" max="5" width="34.1015625" customWidth="1"/>
+    <col min="9" max="9" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.20703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="7">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -1383,11 +1383,11 @@
         <v>27</v>
       </c>
       <c r="D9" s="6">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
         <v>3</v>
       </c>
@@ -1398,11 +1398,11 @@
         <v>29</v>
       </c>
       <c r="D10" s="6">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
         <v>4</v>
       </c>
@@ -1413,11 +1413,11 @@
         <v>32</v>
       </c>
       <c r="D11" s="6">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="7">
         <v>5</v>
       </c>
@@ -1428,11 +1428,11 @@
         <v>35</v>
       </c>
       <c r="D12" s="6">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
         <v>6</v>
       </c>
@@ -1443,11 +1443,11 @@
         <v>38</v>
       </c>
       <c r="D13" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="7">
         <v>7</v>
       </c>
@@ -1458,11 +1458,11 @@
         <v>41</v>
       </c>
       <c r="D14" s="6">
-        <v>220</v>
+        <v>160</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
         <v>8</v>
       </c>
@@ -1473,11 +1473,11 @@
         <v>45</v>
       </c>
       <c r="D15" s="6">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
         <v>22</v>
       </c>
@@ -1557,27 +1557,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22" s="9">
+        <v>8</v>
+      </c>
+      <c r="E22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="9">
-        <v>2</v>
-      </c>
       <c r="F22" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="11" t="s">
         <v>25</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
         <v>41</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="11" t="s">
         <v>42</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="7" t="s">
         <v>26</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="7" t="s">
         <v>16</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
         <v>10</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
         <v>11</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
         <v>12</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
         <v>18</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="7" t="s">
         <v>21</v>
       </c>
@@ -1776,10 +1776,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
@@ -1833,497 +1833,526 @@
       </c>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
+    <row r="43" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="46"/>
       <c r="F44" s="14"/>
     </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31" t="s">
+    <row r="45" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="42"/>
+      <c r="B45" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F45" s="14"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="32" t="s">
+      <c r="D46" s="18"/>
+      <c r="E46" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="31" t="s">
+      <c r="F46" s="40"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="42"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F47" s="19"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="F47" s="40"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="32" t="s">
+      <c r="B48" s="43"/>
+      <c r="C48" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="32" t="s">
+      <c r="D48" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="32" t="s">
+      <c r="E48" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
-      <c r="B49" s="33"/>
-      <c r="C49" s="32" t="s">
+      <c r="F48" s="40"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A49" s="43"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="32" t="s">
+      <c r="D49" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="32" t="s">
+      <c r="E49" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F49" s="19"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="31" t="s">
+      <c r="F49" s="40"/>
+    </row>
+    <row r="50" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="42"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="F50" s="40"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A51" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="32" t="s">
+      <c r="D51" s="18"/>
+      <c r="E51" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="30"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="31" t="s">
+      <c r="F51" s="40"/>
+    </row>
+    <row r="52" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="42"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="31" t="s">
+      <c r="D52" s="19"/>
+      <c r="E52" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F52" s="19"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="25" t="s">
+      <c r="F52" s="40"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A53" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="32" t="s">
+      <c r="B53" s="43"/>
+      <c r="C53" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="25" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="19"/>
-    </row>
-    <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="31" t="s">
+      <c r="F53" s="40"/>
+    </row>
+    <row r="54" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="42"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="19"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+      <c r="D54" s="25"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="40"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A55" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="32" t="s">
+      <c r="B55" s="43"/>
+      <c r="C55" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="32" t="s">
+      <c r="E55" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="F55" s="19"/>
-    </row>
-    <row r="56" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="31" t="s">
+      <c r="F55" s="40"/>
+    </row>
+    <row r="56" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="31" t="s">
+      <c r="E56" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F56" s="19"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="F56" s="40"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A57" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="32" t="s">
+      <c r="B57" s="43"/>
+      <c r="C57" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="32" t="s">
+      <c r="D57" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="30"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="31" t="s">
+      <c r="F57" s="40"/>
+    </row>
+    <row r="58" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="42"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D58" s="35"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="19"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
+      <c r="D58" s="25"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="40"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A59" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="32" t="s">
+      <c r="B59" s="43"/>
+      <c r="C59" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="25" t="s">
+      <c r="D59" s="25"/>
+      <c r="E59" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="F59" s="19"/>
-    </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="30"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="31" t="s">
+      <c r="F59" s="40"/>
+    </row>
+    <row r="60" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="42"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="19"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
+      <c r="D60" s="25"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="40"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A61" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="32" t="s">
+      <c r="B61" s="43"/>
+      <c r="C61" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="32" t="s">
+      <c r="D61" s="25"/>
+      <c r="E61" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="F61" s="19"/>
-    </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="31" t="s">
+      <c r="F61" s="40"/>
+    </row>
+    <row r="62" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="42"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D62" s="34"/>
-      <c r="E62" s="31" t="s">
+      <c r="D62" s="24"/>
+      <c r="E62" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F62" s="19"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F66" s="19"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F67" s="19"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="40"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F66" s="40"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F67" s="40"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F68" s="13"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F69" s="19"/>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F70" s="19"/>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F69" s="40"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F70" s="40"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F71" s="13"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F72" s="19"/>
-    </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F73" s="19"/>
-    </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F74" s="19"/>
-    </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F72" s="40"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F73" s="40"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F74" s="40"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F75" s="13"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F76" s="13"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F77" s="19"/>
-    </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F78" s="19"/>
-    </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F79" s="19"/>
-    </row>
-    <row r="102" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="9:13" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I103" s="39" t="s">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F77" s="40"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F78" s="40"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F79" s="40"/>
+    </row>
+    <row r="102" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="103" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I103" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="J103" s="40" t="s">
+      <c r="J103" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="K103" s="40" t="s">
+      <c r="K103" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="L103" s="41" t="s">
+      <c r="L103" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="M103" s="41" t="s">
+      <c r="M103" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I104" s="46" t="s">
+    <row r="104" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I104" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="J104" s="48" t="s">
+      <c r="J104" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="K104" s="48" t="s">
+      <c r="K104" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L104" s="46" t="s">
+      <c r="L104" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="M104" s="42" t="s">
+      <c r="M104" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="105" spans="9:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I105" s="47"/>
-      <c r="J105" s="49"/>
-      <c r="K105" s="50"/>
-      <c r="L105" s="45"/>
-      <c r="M105" s="43" t="s">
+    <row r="105" spans="9:13" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I105" s="36"/>
+      <c r="J105" s="38"/>
+      <c r="K105" s="39"/>
+      <c r="L105" s="35"/>
+      <c r="M105" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I106" s="44" t="s">
+    <row r="106" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I106" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="J106" s="50"/>
-      <c r="K106" s="43" t="s">
+      <c r="J106" s="39"/>
+      <c r="K106" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="L106" s="47"/>
-      <c r="M106" s="42" t="s">
+      <c r="L106" s="36"/>
+      <c r="M106" s="31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I107" s="46" t="s">
+    <row r="107" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I107" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="J107" s="48" t="s">
+      <c r="J107" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="K107" s="48" t="s">
+      <c r="K107" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="L107" s="46" t="s">
+      <c r="L107" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="M107" s="42" t="s">
+      <c r="M107" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="9:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I108" s="47"/>
-      <c r="J108" s="49"/>
-      <c r="K108" s="50"/>
-      <c r="L108" s="45"/>
-      <c r="M108" s="43" t="s">
+    <row r="108" spans="9:13" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I108" s="36"/>
+      <c r="J108" s="38"/>
+      <c r="K108" s="39"/>
+      <c r="L108" s="35"/>
+      <c r="M108" s="32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I109" s="44" t="s">
+    <row r="109" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I109" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="J109" s="49"/>
-      <c r="K109" s="43" t="s">
+      <c r="J109" s="38"/>
+      <c r="K109" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="L109" s="45"/>
-      <c r="M109" s="43" t="s">
+      <c r="L109" s="35"/>
+      <c r="M109" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I110" s="46" t="s">
+    <row r="110" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I110" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="J110" s="49"/>
-      <c r="K110" s="43" t="s">
+      <c r="J110" s="38"/>
+      <c r="K110" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="L110" s="45"/>
-      <c r="M110" s="46" t="s">
+      <c r="L110" s="35"/>
+      <c r="M110" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I111" s="45"/>
-      <c r="J111" s="49"/>
-      <c r="K111" s="42" t="s">
+    <row r="111" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I111" s="35"/>
+      <c r="J111" s="38"/>
+      <c r="K111" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="L111" s="45"/>
-      <c r="M111" s="45"/>
-    </row>
-    <row r="112" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I112" s="47"/>
-      <c r="J112" s="49"/>
-      <c r="K112" s="43" t="s">
+      <c r="L111" s="35"/>
+      <c r="M111" s="35"/>
+    </row>
+    <row r="112" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I112" s="36"/>
+      <c r="J112" s="38"/>
+      <c r="K112" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="L112" s="45"/>
-      <c r="M112" s="47"/>
-    </row>
-    <row r="113" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I113" s="44" t="s">
+      <c r="L112" s="35"/>
+      <c r="M112" s="36"/>
+    </row>
+    <row r="113" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I113" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="J113" s="49"/>
-      <c r="K113" s="43" t="s">
+      <c r="J113" s="38"/>
+      <c r="K113" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="L113" s="45"/>
-      <c r="M113" s="43" t="s">
+      <c r="L113" s="35"/>
+      <c r="M113" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="9:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I114" s="44" t="s">
+    <row r="114" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I114" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="J114" s="49"/>
-      <c r="K114" s="43" t="s">
+      <c r="J114" s="38"/>
+      <c r="K114" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="L114" s="45"/>
-      <c r="M114" s="43" t="s">
+      <c r="L114" s="35"/>
+      <c r="M114" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I115" s="46" t="s">
+    <row r="115" spans="9:13" ht="27.3" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I115" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="J115" s="49"/>
-      <c r="K115" s="48" t="s">
+      <c r="J115" s="38"/>
+      <c r="K115" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="L115" s="45"/>
-      <c r="M115" s="42" t="s">
+      <c r="L115" s="35"/>
+      <c r="M115" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="9:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I116" s="45"/>
-      <c r="J116" s="49"/>
-      <c r="K116" s="49"/>
-      <c r="L116" s="45"/>
-      <c r="M116" s="43" t="s">
+    <row r="116" spans="9:13" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I116" s="35"/>
+      <c r="J116" s="38"/>
+      <c r="K116" s="38"/>
+      <c r="L116" s="35"/>
+      <c r="M116" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="9:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I117" s="47"/>
-      <c r="J117" s="50"/>
-      <c r="K117" s="50"/>
-      <c r="L117" s="47"/>
-      <c r="M117" s="42" t="s">
+    <row r="117" spans="9:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I117" s="36"/>
+      <c r="J117" s="39"/>
+      <c r="K117" s="39"/>
+      <c r="L117" s="36"/>
+      <c r="M117" s="31" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B62"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="F77:F79"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="J104:J106"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="F72:F74"/>
     <mergeCell ref="M110:M112"/>
     <mergeCell ref="I115:I117"/>
     <mergeCell ref="K115:K117"/>
@@ -2334,35 +2363,6 @@
     <mergeCell ref="K107:K108"/>
     <mergeCell ref="L107:L117"/>
     <mergeCell ref="I110:I112"/>
-    <mergeCell ref="F77:F79"/>
-    <mergeCell ref="I104:I105"/>
-    <mergeCell ref="J104:J106"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="F72:F74"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B62"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A44:A45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2374,197 +2374,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:5" ht="22.2" x14ac:dyDescent="0.4">
+      <c r="A2" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="47" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
+    <row r="3" spans="1:5" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
       <c r="E3" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:5" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="50" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+    <row r="6" spans="1:5" ht="33.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:5" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:5" ht="22.2" x14ac:dyDescent="0.4">
+      <c r="A8" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="49"/>
+      <c r="E8" s="50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5" ht="22.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+    </row>
+    <row r="10" spans="1:5" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="48"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="21.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.4">
+      <c r="A13" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="16" t="s">
+      <c r="B13" s="49"/>
+      <c r="C13" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="32.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+    <row r="14" spans="1:5" ht="33.299999999999997" x14ac:dyDescent="0.4">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+    <row r="15" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="12" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="C13:C15"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C3"/>
@@ -2574,9 +2577,6 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D15"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="C13:C15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2590,7 +2590,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>